<commit_message>
fixed Excel resource file
</commit_message>
<xml_diff>
--- a/Resources/Risky_Business_Tables.xlsx
+++ b/Resources/Risky_Business_Tables.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marshallwolfe/Desktop/Risky_Business/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322FCA33-4128-D74E-86DF-B889F6E9D4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503C8B57-892D-D44A-8201-B2D037D7648A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6360" yWindow="-16100" windowWidth="14340" windowHeight="15880" xr2:uid="{20B7E268-25DF-3046-B5F0-48F160808285}"/>
+    <workbookView xWindow="-7740" yWindow="-28720" windowWidth="14000" windowHeight="9160" xr2:uid="{20B7E268-25DF-3046-B5F0-48F160808285}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,12 +103,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -131,6 +137,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDCFE27-8146-F44F-B94B-99299A8647E8}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -501,7 +508,7 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>0.74</v>
       </c>
       <c r="C4" s="1">
@@ -521,7 +528,7 @@
       <c r="B5" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>0.69</v>
       </c>
       <c r="D5" s="1">
@@ -560,7 +567,7 @@
       <c r="B8" s="1">
         <v>0.64</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>0.65</v>
       </c>
       <c r="D8" s="1">
@@ -577,7 +584,7 @@
       <c r="B9" s="1">
         <v>0.64</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>0.65</v>
       </c>
       <c r="D9" s="1">
@@ -699,43 +706,18 @@
         <v>0.78</v>
       </c>
     </row>
+    <row r="24" spans="1:3">
+      <c r="C24" s="1">
+        <f>6789/C25</f>
+        <v>0.39692469597754909</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" s="1">
+        <v>17104</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:E2">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:E6">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:E10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B14:C14">
     <cfRule type="colorScale" priority="7">
       <colorScale>

</xml_diff>